<commit_message>
Add all Chinese names
</commit_message>
<xml_diff>
--- a/Damage Table.xlsx
+++ b/Damage Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\329058.D007\Desktop\others\16Labs\MHWGB\Monster-Hunter-World-Guide-Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C065B7-90C1-47ED-BE5B-6466D7B0767F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01B540E-015D-44A5-859B-16A3002C0287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9DC5599-DDE8-4A66-810A-B29D278398A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
   <si>
     <t>英文名稱</t>
   </si>
@@ -319,6 +319,102 @@
   </si>
   <si>
     <t>銀火龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>霜刃冰牙龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>金火龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>魚龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰魚龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>泥魚龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>熔岩龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>古龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>貝西摩斯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>剛龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰咒龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>滅盡龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>殲世滅盡龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>屍套龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>霧瘴屍套龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>炎王龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>炎妃龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>麒麟</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冥燈龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>溟波龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天地煌啼龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>絢輝龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冥赤龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>煌黑龍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑龍</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -696,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7AF2C8-D971-4852-B202-CB4F3D2BC098}">
-  <dimension ref="A2:T53"/>
+  <dimension ref="A2:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1033,83 +1129,307 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="2" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C40" s="2" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="2" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="2" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="2" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C44" s="2" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="2" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C46" s="2" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C47" s="2" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C48" s="2" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="2" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="2" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="2" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" s="2" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="2" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add all English name
</commit_message>
<xml_diff>
--- a/Damage Table.xlsx
+++ b/Damage Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\329058.D007\Desktop\others\16Labs\MHWGB\Monster-Hunter-World-Guide-Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4127F6A-817E-407A-BFAB-61C74AECDD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13248F5-7371-46A8-AFBE-421E3E29E9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9DC5599-DDE8-4A66-810A-B29D278398A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="170">
   <si>
     <t>英文名稱</t>
   </si>
@@ -427,6 +427,286 @@
   </si>
   <si>
     <t>古代鹿首精</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ancient Leshen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leshen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fatalis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kulu Ya Ku</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pukei Pukei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coral Pukei Pukei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tzitzi Ya Ku</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yian Garuga</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scarred Yian Garuga</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anjanath</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fulgur Anjanath</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Banbaro</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Barroth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deviljho</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Savage Deviljho</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glavenus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acidic Glavenus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radobaan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uragaan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brachydios</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raging Brachydios</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rajang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Furious Rajang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dodogama</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Great Girros</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Great Jagras</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Odogaron</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ebony Odogaron</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tobi Kadachi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Viper Tobi Kadachi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zinogre</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stygian Zinogre</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Barioth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frostfang Barioth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bazelgeuse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seething Bazelgeuse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diablos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black Diablos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Legiana</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shrieking Legiana</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nargacuga</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paolumu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nightshade Paolumu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rathalos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Azure Rathalos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rathian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pink Rathian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tigrex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brute Tigrex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Silver Rathalos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gold Rathian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beotodus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jyuratodus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lavasioth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behemoth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kushala Daora</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Velkhana</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nergigante</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ruiner Nergigante</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vaal Hazak</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>blackveil Vaal Hazak</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teostra</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lunastra</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kirin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xeno'jiiva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Namielle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sharalshvalda</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kulve Taroth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Safi'jiiva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alatreon</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -816,14 +1096,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7AF2C8-D971-4852-B202-CB4F3D2BC098}">
   <dimension ref="A2:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="11.375" style="2" bestFit="1" customWidth="1"/>
@@ -914,6 +1194,9 @@
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
@@ -922,6 +1205,9 @@
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
@@ -930,6 +1216,9 @@
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
@@ -938,6 +1227,9 @@
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -946,6 +1238,9 @@
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
@@ -954,6 +1249,9 @@
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
@@ -962,6 +1260,9 @@
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
@@ -970,6 +1271,9 @@
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
@@ -978,6 +1282,9 @@
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
@@ -986,6 +1293,9 @@
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
@@ -994,6 +1304,9 @@
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1002,6 +1315,9 @@
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1010,6 +1326,9 @@
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B20" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1018,6 +1337,9 @@
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1026,6 +1348,9 @@
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1034,6 +1359,9 @@
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B23" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1042,6 +1370,9 @@
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1050,6 +1381,9 @@
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1058,6 +1392,9 @@
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B26" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>43</v>
       </c>
@@ -1066,6 +1403,9 @@
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>44</v>
       </c>
@@ -1074,6 +1414,9 @@
       <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B28" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
@@ -1082,6 +1425,9 @@
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="C29" s="2" t="s">
         <v>47</v>
       </c>
@@ -1090,6 +1436,9 @@
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="C30" s="2" t="s">
         <v>48</v>
       </c>
@@ -1098,6 +1447,9 @@
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B31" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>49</v>
       </c>
@@ -1106,6 +1458,9 @@
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B32" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
@@ -1114,6 +1469,9 @@
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B33" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="C33" s="2" t="s">
         <v>51</v>
       </c>
@@ -1122,6 +1480,9 @@
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B34" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="C34" s="2" t="s">
         <v>52</v>
       </c>
@@ -1130,6 +1491,9 @@
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B35" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
@@ -1138,6 +1502,9 @@
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="C36" s="2" t="s">
         <v>54</v>
       </c>
@@ -1146,6 +1513,9 @@
       <c r="A37" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B37" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
@@ -1154,6 +1524,9 @@
       <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B38" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>73</v>
       </c>
@@ -1162,6 +1535,9 @@
       <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B39" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="C39" s="2" t="s">
         <v>57</v>
       </c>
@@ -1170,6 +1546,9 @@
       <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B40" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="C40" s="2" t="s">
         <v>58</v>
       </c>
@@ -1178,6 +1557,9 @@
       <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B41" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="C41" s="2" t="s">
         <v>59</v>
       </c>
@@ -1186,6 +1568,9 @@
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B42" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="C42" s="2" t="s">
         <v>60</v>
       </c>
@@ -1194,6 +1579,9 @@
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B43" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="C43" s="2" t="s">
         <v>61</v>
       </c>
@@ -1202,6 +1590,9 @@
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B44" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="C44" s="2" t="s">
         <v>62</v>
       </c>
@@ -1210,6 +1601,9 @@
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B45" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="C45" s="2" t="s">
         <v>63</v>
       </c>
@@ -1218,6 +1612,9 @@
       <c r="A46" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B46" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="C46" s="2" t="s">
         <v>64</v>
       </c>
@@ -1226,6 +1623,9 @@
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B47" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="C47" s="2" t="s">
         <v>65</v>
       </c>
@@ -1234,6 +1634,9 @@
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B48" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="C48" s="2" t="s">
         <v>66</v>
       </c>
@@ -1242,6 +1645,9 @@
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B49" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="C49" s="2" t="s">
         <v>67</v>
       </c>
@@ -1250,6 +1656,9 @@
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B50" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="C50" s="2" t="s">
         <v>69</v>
       </c>
@@ -1258,6 +1667,9 @@
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B51" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="C51" s="2" t="s">
         <v>68</v>
       </c>
@@ -1266,6 +1678,9 @@
       <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B52" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="C52" s="2" t="s">
         <v>70</v>
       </c>
@@ -1274,6 +1689,9 @@
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B53" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="C53" s="2" t="s">
         <v>71</v>
       </c>
@@ -1282,6 +1700,9 @@
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B54" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="C54" s="2" t="s">
         <v>72</v>
       </c>
@@ -1290,6 +1711,9 @@
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B55" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="C55" s="2" t="s">
         <v>74</v>
       </c>
@@ -1298,6 +1722,9 @@
       <c r="A56" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="B56" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="C56" s="2" t="s">
         <v>76</v>
       </c>
@@ -1306,6 +1733,9 @@
       <c r="A57" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="B57" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="C57" s="2" t="s">
         <v>77</v>
       </c>
@@ -1314,6 +1744,9 @@
       <c r="A58" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="B58" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="C58" s="2" t="s">
         <v>78</v>
       </c>
@@ -1322,6 +1755,9 @@
       <c r="A59" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B59" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="C59" s="2" t="s">
         <v>80</v>
       </c>
@@ -1330,6 +1766,9 @@
       <c r="A60" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B60" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="C60" s="2" t="s">
         <v>81</v>
       </c>
@@ -1338,6 +1777,9 @@
       <c r="A61" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B61" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="C61" s="2" t="s">
         <v>82</v>
       </c>
@@ -1346,6 +1788,9 @@
       <c r="A62" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B62" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="C62" s="2" t="s">
         <v>83</v>
       </c>
@@ -1354,6 +1799,9 @@
       <c r="A63" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B63" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="C63" s="2" t="s">
         <v>84</v>
       </c>
@@ -1362,6 +1810,9 @@
       <c r="A64" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B64" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="C64" s="2" t="s">
         <v>85</v>
       </c>
@@ -1370,6 +1821,9 @@
       <c r="A65" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B65" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="C65" s="2" t="s">
         <v>86</v>
       </c>
@@ -1378,6 +1832,9 @@
       <c r="A66" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B66" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="C66" s="2" t="s">
         <v>87</v>
       </c>
@@ -1386,6 +1843,9 @@
       <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B67" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="C67" s="2" t="s">
         <v>88</v>
       </c>
@@ -1394,6 +1854,9 @@
       <c r="A68" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B68" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="C68" s="2" t="s">
         <v>89</v>
       </c>
@@ -1402,6 +1865,9 @@
       <c r="A69" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B69" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="C69" s="2" t="s">
         <v>90</v>
       </c>
@@ -1410,6 +1876,9 @@
       <c r="A70" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B70" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="C70" s="2" t="s">
         <v>91</v>
       </c>
@@ -1418,6 +1887,9 @@
       <c r="A71" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B71" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="C71" s="2" t="s">
         <v>92</v>
       </c>
@@ -1426,6 +1898,9 @@
       <c r="A72" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B72" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="C72" s="2" t="s">
         <v>93</v>
       </c>
@@ -1434,6 +1909,9 @@
       <c r="A73" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B73" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="C73" s="2" t="s">
         <v>94</v>
       </c>
@@ -1442,6 +1920,9 @@
       <c r="A74" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B74" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="C74" s="2" t="s">
         <v>95</v>
       </c>
@@ -1450,6 +1931,9 @@
       <c r="A75" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B75" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C75" s="2" t="s">
         <v>96</v>
       </c>
@@ -1458,6 +1942,9 @@
       <c r="A76" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="B76" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="C76" s="2" t="s">
         <v>98</v>
       </c>
@@ -1465,6 +1952,9 @@
     <row r="77" spans="1:3">
       <c r="A77" s="3" t="s">
         <v>97</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Add all Pukei Pukei
</commit_message>
<xml_diff>
--- a/Damage Table.xlsx
+++ b/Damage Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\329058.D007\Desktop\others\16Labs\MHWGB\Monster-Hunter-World-Guide-Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A839BC-FDCD-48C1-BE08-538CC2ADFC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC4DA4E-C44E-4C31-826A-5005DFBEA4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9DC5599-DDE8-4A66-810A-B29D278398A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="197">
   <si>
     <t>英文名稱</t>
   </si>
@@ -769,11 +769,55 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>擊暈</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>爆炸石存在其他強力派生攻擊，如:爆炸投擲、地雷等附加火屬性且高傷害之技能，由於爆炸石本身出現條件嚴苛，故暫且不計</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吐舌攻擊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>毒彈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>毒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓄力毒彈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水球</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓄力水球</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水鐵炮</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水鐵炮(大)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水鐵炮(必殺)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>掃射水流</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>掃射水流(大)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -845,7 +889,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -859,6 +903,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1185,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7AF2C8-D971-4852-B202-CB4F3D2BC098}">
-  <dimension ref="A2:AJ394"/>
+  <dimension ref="A2:AJ405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1269,63 +1316,63 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:36">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7" t="s">
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7" t="s">
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7" t="s">
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7" t="s">
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7" t="s">
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7" t="s">
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
-      <c r="AG6" s="7" t="s">
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
     </row>
     <row r="7" spans="1:36">
       <c r="A7" s="2" t="s">
@@ -1472,99 +1519,99 @@
         <v>0</v>
       </c>
       <c r="L8" s="2">
-        <f>E8*I8</f>
+        <f t="shared" ref="L8:L14" si="0">E8*I8</f>
         <v>192</v>
       </c>
       <c r="M8" s="2">
-        <f>E8*J8</f>
+        <f t="shared" ref="M8:M14" si="1">E8*J8</f>
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <f>E8*K8</f>
+        <f t="shared" ref="N8:N14" si="2">E8*K8</f>
         <v>0</v>
       </c>
       <c r="O8" s="5">
-        <f>F8*I8</f>
+        <f t="shared" ref="O8:O14" si="3">F8*I8</f>
         <v>264</v>
       </c>
       <c r="P8" s="5">
-        <f>F8*J8</f>
+        <f t="shared" ref="P8:P14" si="4">F8*J8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="5">
-        <f>F8*K8</f>
+        <f t="shared" ref="Q8:Q14" si="5">F8*K8</f>
         <v>0</v>
       </c>
       <c r="R8" s="5">
-        <f>H8*I8</f>
+        <f t="shared" ref="R8:R14" si="6">H8*I8</f>
         <v>0</v>
       </c>
       <c r="S8" s="5">
-        <f>H8*J8</f>
+        <f t="shared" ref="S8:S14" si="7">H8*J8</f>
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <f>H8*K8</f>
+        <f t="shared" ref="T8:T14" si="8">H8*K8</f>
         <v>0</v>
       </c>
       <c r="U8" s="4">
-        <f>L8*$G$3/$E$3</f>
+        <f t="shared" ref="U8:W14" si="9">L8*$G$3/$E$3</f>
         <v>9.481481481481481E-2</v>
       </c>
       <c r="V8" s="4">
-        <f>M8*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W8" s="4">
-        <f>N8*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X8" s="4">
-        <f>R8*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" ref="X8:Z14" si="10">R8*$G$3*(1-$H$3)/$E$3</f>
         <v>0</v>
       </c>
       <c r="Y8" s="4">
-        <f>S8*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z8" s="4">
-        <f>T8*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AA8" s="4">
-        <f>O8*$G$3/$E$3</f>
+        <f t="shared" ref="AA8:AC14" si="11">O8*$G$3/$E$3</f>
         <v>0.13037037037037036</v>
       </c>
       <c r="AB8" s="4">
-        <f>P8*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC8" s="4">
-        <f>Q8*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD8" s="2" t="str">
-        <f t="shared" ref="AD8:AI8" si="0">IF((U8+X8)&lt;($J$4/2),"低",IF((U8+X8)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AD8:AI8" si="12">IF((U8+X8)&lt;($J$4/2),"低",IF((U8+X8)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AE8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>低</v>
       </c>
       <c r="AF8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>低</v>
       </c>
       <c r="AG8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>低</v>
       </c>
       <c r="AH8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>低</v>
       </c>
       <c r="AI8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>低</v>
       </c>
     </row>
@@ -1578,8 +1625,8 @@
       <c r="F9" s="6">
         <v>45</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>184</v>
+      <c r="G9" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="H9" s="6">
         <v>0</v>
@@ -1594,99 +1641,99 @@
         <v>0</v>
       </c>
       <c r="L9" s="6">
-        <f>E9*I9</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="M9" s="6">
-        <f>E9*J9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N9" s="6">
-        <f>E9*K9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O9" s="6">
-        <f>F9*I9</f>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="P9" s="6">
-        <f>F9*J9</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q9" s="6">
-        <f>F9*K9</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R9" s="6">
-        <f>H9*I9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S9" s="6">
-        <f>H9*J9</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T9" s="6">
-        <f>H9*K9</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U9" s="4">
-        <f>L9*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0.12641975308641976</v>
       </c>
       <c r="V9" s="4">
-        <f>M9*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W9" s="4">
-        <f>N9*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X9" s="4">
-        <f>R9*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y9" s="4">
-        <f>S9*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z9" s="4">
-        <f>T9*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AA9" s="4">
-        <f>O9*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0.17777777777777776</v>
       </c>
       <c r="AB9" s="4">
-        <f>P9*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC9" s="4">
-        <f>Q9*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD9" s="6" t="str">
-        <f t="shared" ref="AD9" si="1">IF((U9+X9)&lt;($J$4/2),"低",IF((U9+X9)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AD9" si="13">IF((U9+X9)&lt;($J$4/2),"低",IF((U9+X9)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AE9" s="6" t="str">
-        <f t="shared" ref="AE9" si="2">IF((V9+Y9)&lt;($J$4/2),"低",IF((V9+Y9)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AE9" si="14">IF((V9+Y9)&lt;($J$4/2),"低",IF((V9+Y9)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AF9" s="6" t="str">
-        <f t="shared" ref="AF9" si="3">IF((W9+Z9)&lt;($J$4/2),"低",IF((W9+Z9)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AF9" si="15">IF((W9+Z9)&lt;($J$4/2),"低",IF((W9+Z9)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AG9" s="6" t="str">
-        <f t="shared" ref="AG9" si="4">IF((X9+AA9)&lt;($J$4/2),"低",IF((X9+AA9)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AG9" si="16">IF((X9+AA9)&lt;($J$4/2),"低",IF((X9+AA9)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AH9" s="6" t="str">
-        <f t="shared" ref="AH9" si="5">IF((Y9+AB9)&lt;($J$4/2),"低",IF((Y9+AB9)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AH9" si="17">IF((Y9+AB9)&lt;($J$4/2),"低",IF((Y9+AB9)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AI9" s="6" t="str">
-        <f t="shared" ref="AI9" si="6">IF((Z9+AC9)&lt;($J$4/2),"低",IF((Z9+AC9)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AI9" si="18">IF((Z9+AC9)&lt;($J$4/2),"低",IF((Z9+AC9)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
     </row>
@@ -1700,8 +1747,8 @@
       <c r="F10" s="6">
         <v>90</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>184</v>
+      <c r="G10" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="H10" s="6">
         <v>0</v>
@@ -1716,99 +1763,99 @@
         <v>0</v>
       </c>
       <c r="L10" s="6">
-        <f>E10*I10</f>
+        <f t="shared" si="0"/>
         <v>520</v>
       </c>
       <c r="M10" s="6">
-        <f>E10*J10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N10" s="6">
-        <f>E10*K10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O10" s="6">
-        <f>F10*I10</f>
+        <f t="shared" si="3"/>
         <v>720</v>
       </c>
       <c r="P10" s="6">
-        <f>F10*J10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q10" s="6">
-        <f>F10*K10</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R10" s="6">
-        <f>H10*I10</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S10" s="6">
-        <f>H10*J10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T10" s="6">
-        <f>H10*K10</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U10" s="4">
-        <f>L10*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0.25679012345679014</v>
       </c>
       <c r="V10" s="4">
-        <f>M10*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W10" s="4">
-        <f>N10*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X10" s="4">
-        <f>R10*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y10" s="4">
-        <f>S10*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z10" s="4">
-        <f>T10*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AA10" s="4">
-        <f>O10*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0.35555555555555551</v>
       </c>
       <c r="AB10" s="4">
-        <f>P10*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC10" s="4">
-        <f>Q10*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD10" s="6" t="str">
-        <f t="shared" ref="AD10:AD12" si="7">IF((U10+X10)&lt;($J$4/2),"低",IF((U10+X10)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AD10:AD12" si="19">IF((U10+X10)&lt;($J$4/2),"低",IF((U10+X10)&gt;$J$4,"高","中"))</f>
         <v>中</v>
       </c>
       <c r="AE10" s="6" t="str">
-        <f t="shared" ref="AE10:AE12" si="8">IF((V10+Y10)&lt;($J$4/2),"低",IF((V10+Y10)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AE10:AE12" si="20">IF((V10+Y10)&lt;($J$4/2),"低",IF((V10+Y10)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AF10" s="6" t="str">
-        <f t="shared" ref="AF10:AF12" si="9">IF((W10+Z10)&lt;($J$4/2),"低",IF((W10+Z10)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AF10:AF12" si="21">IF((W10+Z10)&lt;($J$4/2),"低",IF((W10+Z10)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AG10" s="6" t="str">
-        <f t="shared" ref="AG10:AG12" si="10">IF((X10+AA10)&lt;($J$4/2),"低",IF((X10+AA10)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AG10:AG12" si="22">IF((X10+AA10)&lt;($J$4/2),"低",IF((X10+AA10)&gt;$J$4,"高","中"))</f>
         <v>中</v>
       </c>
       <c r="AH10" s="6" t="str">
-        <f t="shared" ref="AH10:AH12" si="11">IF((Y10+AB10)&lt;($J$4/2),"低",IF((Y10+AB10)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AH10:AH12" si="23">IF((Y10+AB10)&lt;($J$4/2),"低",IF((Y10+AB10)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AI10" s="6" t="str">
-        <f t="shared" ref="AI10:AI12" si="12">IF((Z10+AC10)&lt;($J$4/2),"低",IF((Z10+AC10)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AI10:AI12" si="24">IF((Z10+AC10)&lt;($J$4/2),"低",IF((Z10+AC10)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
     </row>
@@ -1838,99 +1885,99 @@
         <v>0</v>
       </c>
       <c r="L11" s="6">
-        <f>E11*I11</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="M11" s="6">
-        <f>E11*J11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11" s="6">
-        <f>E11*K11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O11" s="6">
-        <f>F11*I11</f>
+        <f t="shared" si="3"/>
         <v>224</v>
       </c>
       <c r="P11" s="6">
-        <f>F11*J11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q11" s="6">
-        <f>F11*K11</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R11" s="6">
-        <f>H11*I11</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S11" s="6">
-        <f>H11*J11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T11" s="6">
-        <f>H11*K11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U11" s="4">
-        <f>L11*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>7.9012345679012344E-2</v>
       </c>
       <c r="V11" s="4">
-        <f>M11*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W11" s="4">
-        <f>N11*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X11" s="4">
-        <f>R11*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y11" s="4">
-        <f>S11*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z11" s="4">
-        <f>T11*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AA11" s="4">
-        <f>O11*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0.11061728395061728</v>
       </c>
       <c r="AB11" s="4">
-        <f>P11*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC11" s="4">
-        <f>Q11*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD11" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>低</v>
       </c>
       <c r="AE11" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="20"/>
         <v>低</v>
       </c>
       <c r="AF11" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>低</v>
       </c>
       <c r="AG11" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>低</v>
       </c>
       <c r="AH11" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="23"/>
         <v>低</v>
       </c>
       <c r="AI11" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>低</v>
       </c>
     </row>
@@ -1944,8 +1991,8 @@
       <c r="F12" s="6">
         <v>50</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>184</v>
+      <c r="G12" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="H12" s="6">
         <v>0</v>
@@ -1960,103 +2007,103 @@
         <v>0</v>
       </c>
       <c r="L12" s="6">
-        <f>E12*I12</f>
+        <f t="shared" si="0"/>
         <v>288</v>
       </c>
       <c r="M12" s="6">
-        <f>E12*J12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12" s="6">
-        <f>E12*K12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O12" s="6">
-        <f>F12*I12</f>
+        <f t="shared" si="3"/>
         <v>400</v>
       </c>
       <c r="P12" s="6">
-        <f>F12*J12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q12" s="6">
-        <f>F12*K12</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R12" s="6">
-        <f>H12*I12</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S12" s="6">
-        <f>H12*J12</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="6">
-        <f>H12*K12</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U12" s="4">
-        <f>L12*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0.14222222222222222</v>
       </c>
       <c r="V12" s="4">
-        <f>M12*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W12" s="4">
-        <f>N12*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X12" s="4">
-        <f>R12*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y12" s="4">
-        <f>S12*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z12" s="4">
-        <f>T12*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AA12" s="4">
-        <f>O12*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="AB12" s="4">
-        <f>P12*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC12" s="4">
-        <f>Q12*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD12" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>低</v>
       </c>
       <c r="AE12" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="20"/>
         <v>低</v>
       </c>
       <c r="AF12" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>低</v>
       </c>
       <c r="AG12" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>低</v>
       </c>
       <c r="AH12" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="23"/>
         <v>低</v>
       </c>
       <c r="AI12" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>低</v>
       </c>
       <c r="AJ12" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:36" s="6" customFormat="1">
@@ -2069,8 +2116,8 @@
       <c r="F13" s="6">
         <v>56</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>184</v>
+      <c r="G13" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="H13" s="6">
         <v>0</v>
@@ -2085,99 +2132,99 @@
         <v>0</v>
       </c>
       <c r="L13" s="6">
-        <f>E13*I13</f>
+        <f t="shared" si="0"/>
         <v>320</v>
       </c>
       <c r="M13" s="6">
-        <f>E13*J13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13" s="6">
-        <f>E13*K13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13" s="6">
-        <f>F13*I13</f>
+        <f t="shared" si="3"/>
         <v>448</v>
       </c>
       <c r="P13" s="6">
-        <f>F13*J13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q13" s="6">
-        <f>F13*K13</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R13" s="6">
-        <f>H13*I13</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S13" s="6">
-        <f>H13*J13</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T13" s="6">
-        <f>H13*K13</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U13" s="4">
-        <f>L13*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0.15802469135802469</v>
       </c>
       <c r="V13" s="4">
-        <f>M13*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W13" s="4">
-        <f>N13*$G$3/$E$3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X13" s="4">
-        <f>R13*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y13" s="4">
-        <f>S13*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z13" s="4">
-        <f>T13*$G$3*(1-$H$3)/$E$3</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AA13" s="4">
-        <f>O13*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0.22123456790123455</v>
       </c>
       <c r="AB13" s="4">
-        <f>P13*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC13" s="4">
-        <f>Q13*$G$3/$E$3</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD13" s="6" t="str">
-        <f t="shared" ref="AD13" si="13">IF((U13+X13)&lt;($J$4/2),"低",IF((U13+X13)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AD13:AD14" si="25">IF((U13+X13)&lt;($J$4/2),"低",IF((U13+X13)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AE13" s="6" t="str">
-        <f t="shared" ref="AE13" si="14">IF((V13+Y13)&lt;($J$4/2),"低",IF((V13+Y13)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AE13:AE14" si="26">IF((V13+Y13)&lt;($J$4/2),"低",IF((V13+Y13)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AF13" s="6" t="str">
-        <f t="shared" ref="AF13" si="15">IF((W13+Z13)&lt;($J$4/2),"低",IF((W13+Z13)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AF13:AF14" si="27">IF((W13+Z13)&lt;($J$4/2),"低",IF((W13+Z13)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AG13" s="6" t="str">
-        <f t="shared" ref="AG13" si="16">IF((X13+AA13)&lt;($J$4/2),"低",IF((X13+AA13)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AG13:AG14" si="28">IF((X13+AA13)&lt;($J$4/2),"低",IF((X13+AA13)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AH13" s="6" t="str">
-        <f t="shared" ref="AH13" si="17">IF((Y13+AB13)&lt;($J$4/2),"低",IF((Y13+AB13)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AH13:AH14" si="29">IF((Y13+AB13)&lt;($J$4/2),"低",IF((Y13+AB13)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
       <c r="AI13" s="6" t="str">
-        <f t="shared" ref="AI13" si="18">IF((Z13+AC13)&lt;($J$4/2),"低",IF((Z13+AC13)&gt;$J$4,"高","中"))</f>
+        <f t="shared" ref="AI13:AI14" si="30">IF((Z13+AC13)&lt;($J$4/2),"低",IF((Z13+AC13)&gt;$J$4,"高","中"))</f>
         <v>低</v>
       </c>
     </row>
@@ -2191,265 +2238,1609 @@
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-    </row>
-    <row r="15" spans="1:36">
-      <c r="A15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-    </row>
-    <row r="16" spans="1:36">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-    </row>
-    <row r="17" spans="1:29">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
-    </row>
-    <row r="18" spans="1:29">
+      <c r="D14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="2">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2">
+        <v>33</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" si="3"/>
+        <v>313.5</v>
+      </c>
+      <c r="P14" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11259259259259259</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="4">
+        <f t="shared" si="11"/>
+        <v>0.15481481481481482</v>
+      </c>
+      <c r="AB14" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>低</v>
+      </c>
+      <c r="AE14" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>低</v>
+      </c>
+      <c r="AF14" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>低</v>
+      </c>
+      <c r="AG14" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>低</v>
+      </c>
+      <c r="AH14" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>低</v>
+      </c>
+      <c r="AI14" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" s="7" customFormat="1">
+      <c r="D15" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="7">
+        <v>44</v>
+      </c>
+      <c r="F15" s="7">
+        <v>62</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" ref="L15" si="31">E15*I15</f>
+        <v>418</v>
+      </c>
+      <c r="M15" s="7">
+        <f t="shared" ref="M15" si="32">E15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <f t="shared" ref="N15" si="33">E15*K15</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
+        <f t="shared" ref="O15" si="34">F15*I15</f>
+        <v>589</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" ref="P15" si="35">F15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" ref="Q15" si="36">F15*K15</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
+        <f t="shared" ref="R15" si="37">H15*I15</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="7">
+        <f t="shared" ref="S15" si="38">H15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="7">
+        <f t="shared" ref="T15" si="39">H15*K15</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" ref="U15" si="40">L15*$G$3/$E$3</f>
+        <v>0.20641975308641974</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" ref="V15" si="41">M15*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="4">
+        <f t="shared" ref="W15" si="42">N15*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
+        <f t="shared" ref="X15" si="43">R15*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="4">
+        <f t="shared" ref="Y15" si="44">S15*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="4">
+        <f t="shared" ref="Z15" si="45">T15*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="4">
+        <f t="shared" ref="AA15" si="46">O15*$G$3/$E$3</f>
+        <v>0.29086419753086418</v>
+      </c>
+      <c r="AB15" s="4">
+        <f t="shared" ref="AB15" si="47">P15*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="4">
+        <f t="shared" ref="AC15" si="48">Q15*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="7" t="str">
+        <f t="shared" ref="AD15" si="49">IF((U15+X15)&lt;($J$4/2),"低",IF((U15+X15)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AE15" s="7" t="str">
+        <f t="shared" ref="AE15" si="50">IF((V15+Y15)&lt;($J$4/2),"低",IF((V15+Y15)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AF15" s="7" t="str">
+        <f t="shared" ref="AF15" si="51">IF((W15+Z15)&lt;($J$4/2),"低",IF((W15+Z15)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG15" s="7" t="str">
+        <f t="shared" ref="AG15" si="52">IF((X15+AA15)&lt;($J$4/2),"低",IF((X15+AA15)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH15" s="7" t="str">
+        <f t="shared" ref="AH15" si="53">IF((Y15+AB15)&lt;($J$4/2),"低",IF((Y15+AB15)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AI15" s="7" t="str">
+        <f t="shared" ref="AI15" si="54">IF((Z15+AC15)&lt;($J$4/2),"低",IF((Z15+AC15)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" s="7" customFormat="1">
+      <c r="D16" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E16" s="7">
+        <v>16</v>
+      </c>
+      <c r="F16" s="7">
+        <v>22</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" ref="L16" si="55">E16*I16</f>
+        <v>152</v>
+      </c>
+      <c r="M16" s="7">
+        <f t="shared" ref="M16" si="56">E16*J16</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <f t="shared" ref="N16" si="57">E16*K16</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
+        <f t="shared" ref="O16" si="58">F16*I16</f>
+        <v>209</v>
+      </c>
+      <c r="P16" s="7">
+        <f t="shared" ref="P16" si="59">F16*J16</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" ref="Q16" si="60">F16*K16</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="7">
+        <f t="shared" ref="R16" si="61">H16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" ref="S16" si="62">H16*J16</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="7">
+        <f t="shared" ref="T16" si="63">H16*K16</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" ref="U16" si="64">L16*$G$3/$E$3</f>
+        <v>7.5061728395061728E-2</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" ref="V16" si="65">M16*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="4">
+        <f t="shared" ref="W16" si="66">N16*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="4">
+        <f t="shared" ref="X16" si="67">R16*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="4">
+        <f t="shared" ref="Y16" si="68">S16*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="4">
+        <f t="shared" ref="Z16" si="69">T16*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="4">
+        <f t="shared" ref="AA16" si="70">O16*$G$3/$E$3</f>
+        <v>0.10320987654320987</v>
+      </c>
+      <c r="AB16" s="4">
+        <f t="shared" ref="AB16" si="71">P16*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="4">
+        <f t="shared" ref="AC16" si="72">Q16*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="7" t="str">
+        <f t="shared" ref="AD16" si="73">IF((U16+X16)&lt;($J$4/2),"低",IF((U16+X16)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AE16" s="7" t="str">
+        <f t="shared" ref="AE16" si="74">IF((V16+Y16)&lt;($J$4/2),"低",IF((V16+Y16)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AF16" s="7" t="str">
+        <f t="shared" ref="AF16" si="75">IF((W16+Z16)&lt;($J$4/2),"低",IF((W16+Z16)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG16" s="7" t="str">
+        <f t="shared" ref="AG16" si="76">IF((X16+AA16)&lt;($J$4/2),"低",IF((X16+AA16)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AH16" s="7" t="str">
+        <f t="shared" ref="AH16" si="77">IF((Y16+AB16)&lt;($J$4/2),"低",IF((Y16+AB16)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AI16" s="7" t="str">
+        <f t="shared" ref="AI16" si="78">IF((Z16+AC16)&lt;($J$4/2),"低",IF((Z16+AC16)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" s="7" customFormat="1">
+      <c r="D17" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="7">
+        <v>44</v>
+      </c>
+      <c r="F17" s="7">
+        <v>62</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" ref="L17:L18" si="79">E17*I17</f>
+        <v>418</v>
+      </c>
+      <c r="M17" s="7">
+        <f t="shared" ref="M17:M18" si="80">E17*J17</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <f t="shared" ref="N17:N18" si="81">E17*K17</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <f t="shared" ref="O17:O27" si="82">F17*I17</f>
+        <v>589</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" ref="P17:P18" si="83">F17*J17</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
+        <f t="shared" ref="Q17:Q18" si="84">F17*K17</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="7">
+        <f t="shared" ref="R17:R18" si="85">H17*I17</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="7">
+        <f t="shared" ref="S17:S18" si="86">H17*J17</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="7">
+        <f t="shared" ref="T17:T18" si="87">H17*K17</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" ref="U17:U18" si="88">L17*$G$3/$E$3</f>
+        <v>0.20641975308641974</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" ref="V17:V18" si="89">M17*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" ref="W17:W18" si="90">N17*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" ref="X17:X18" si="91">R17*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="4">
+        <f t="shared" ref="Y17:Y18" si="92">S17*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="4">
+        <f t="shared" ref="Z17:Z18" si="93">T17*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="4">
+        <f t="shared" ref="AA17:AA18" si="94">O17*$G$3/$E$3</f>
+        <v>0.29086419753086418</v>
+      </c>
+      <c r="AB17" s="4">
+        <f t="shared" ref="AB17:AB18" si="95">P17*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="4">
+        <f t="shared" ref="AC17:AC18" si="96">Q17*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="7" t="str">
+        <f t="shared" ref="AD17:AD18" si="97">IF((U17+X17)&lt;($J$4/2),"低",IF((U17+X17)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AE17" s="7" t="str">
+        <f t="shared" ref="AE17:AE18" si="98">IF((V17+Y17)&lt;($J$4/2),"低",IF((V17+Y17)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AF17" s="7" t="str">
+        <f t="shared" ref="AF17:AF18" si="99">IF((W17+Z17)&lt;($J$4/2),"低",IF((W17+Z17)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG17" s="7" t="str">
+        <f t="shared" ref="AG17:AG18" si="100">IF((X17+AA17)&lt;($J$4/2),"低",IF((X17+AA17)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH17" s="7" t="str">
+        <f t="shared" ref="AH17:AH18" si="101">IF((Y17+AB17)&lt;($J$4/2),"低",IF((Y17+AB17)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AI17" s="7" t="str">
+        <f t="shared" ref="AI17:AI18" si="102">IF((Z17+AC17)&lt;($J$4/2),"低",IF((Z17+AC17)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
-    </row>
-    <row r="19" spans="1:29">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
-    </row>
-    <row r="20" spans="1:29">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
-    </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-    </row>
-    <row r="22" spans="1:29">
-      <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
-    </row>
-    <row r="23" spans="1:29">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
-    </row>
-    <row r="24" spans="1:29">
-      <c r="A24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
-    </row>
-    <row r="25" spans="1:29">
-      <c r="A25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="7">
         <v>24</v>
       </c>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-    </row>
-    <row r="26" spans="1:29">
-      <c r="A26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
-    </row>
-    <row r="27" spans="1:29">
+      <c r="F18" s="7">
+        <v>33</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>7</v>
+      </c>
+      <c r="J18" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="79"/>
+        <v>168</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="80"/>
+        <v>252</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="81"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="7">
+        <f t="shared" si="82"/>
+        <v>231</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" si="83"/>
+        <v>346.5</v>
+      </c>
+      <c r="Q18" s="5">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="7">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="5">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="87"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="88"/>
+        <v>8.2962962962962947E-2</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="89"/>
+        <v>0.12444444444444443</v>
+      </c>
+      <c r="W18" s="4">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="4">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="4">
+        <f t="shared" si="92"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="4">
+        <f t="shared" si="93"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="4">
+        <f t="shared" si="94"/>
+        <v>0.11407407407407408</v>
+      </c>
+      <c r="AB18" s="4">
+        <f t="shared" si="95"/>
+        <v>0.1711111111111111</v>
+      </c>
+      <c r="AC18" s="4">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="7" t="str">
+        <f t="shared" si="97"/>
+        <v>低</v>
+      </c>
+      <c r="AE18" s="2" t="str">
+        <f t="shared" si="98"/>
+        <v>低</v>
+      </c>
+      <c r="AF18" s="2" t="str">
+        <f t="shared" si="99"/>
+        <v>低</v>
+      </c>
+      <c r="AG18" s="7" t="str">
+        <f t="shared" si="100"/>
+        <v>低</v>
+      </c>
+      <c r="AH18" s="5" t="str">
+        <f t="shared" si="101"/>
+        <v>低</v>
+      </c>
+      <c r="AI18" s="5" t="str">
+        <f t="shared" si="102"/>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" s="7" customFormat="1">
+      <c r="D19" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" s="7">
+        <v>44</v>
+      </c>
+      <c r="F19" s="7">
+        <v>62</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7">
+        <v>7</v>
+      </c>
+      <c r="J19" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" ref="L19" si="103">E19*I19</f>
+        <v>308</v>
+      </c>
+      <c r="M19" s="7">
+        <f t="shared" ref="M19" si="104">E19*J19</f>
+        <v>462</v>
+      </c>
+      <c r="N19" s="7">
+        <f t="shared" ref="N19" si="105">E19*K19</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="7">
+        <f t="shared" ref="O19" si="106">F19*I19</f>
+        <v>434</v>
+      </c>
+      <c r="P19" s="7">
+        <f t="shared" ref="P19" si="107">F19*J19</f>
+        <v>651</v>
+      </c>
+      <c r="Q19" s="7">
+        <f t="shared" ref="Q19" si="108">F19*K19</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="7">
+        <f t="shared" ref="R19" si="109">H19*I19</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="7">
+        <f t="shared" ref="S19" si="110">H19*J19</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="7">
+        <f t="shared" ref="T19" si="111">H19*K19</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" ref="U19" si="112">L19*$G$3/$E$3</f>
+        <v>0.15209876543209874</v>
+      </c>
+      <c r="V19" s="4">
+        <f t="shared" ref="V19" si="113">M19*$G$3/$E$3</f>
+        <v>0.22814814814814816</v>
+      </c>
+      <c r="W19" s="4">
+        <f t="shared" ref="W19" si="114">N19*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="4">
+        <f t="shared" ref="X19" si="115">R19*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="4">
+        <f t="shared" ref="Y19" si="116">S19*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="4">
+        <f t="shared" ref="Z19" si="117">T19*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="4">
+        <f t="shared" ref="AA19" si="118">O19*$G$3/$E$3</f>
+        <v>0.21432098765432098</v>
+      </c>
+      <c r="AB19" s="4">
+        <f t="shared" ref="AB19" si="119">P19*$G$3/$E$3</f>
+        <v>0.32148148148148148</v>
+      </c>
+      <c r="AC19" s="4">
+        <f t="shared" ref="AC19" si="120">Q19*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="7" t="str">
+        <f t="shared" ref="AD19" si="121">IF((U19+X19)&lt;($J$4/2),"低",IF((U19+X19)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AE19" s="7" t="str">
+        <f t="shared" ref="AE19" si="122">IF((V19+Y19)&lt;($J$4/2),"低",IF((V19+Y19)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AF19" s="7" t="str">
+        <f t="shared" ref="AF19" si="123">IF((W19+Z19)&lt;($J$4/2),"低",IF((W19+Z19)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG19" s="7" t="str">
+        <f t="shared" ref="AG19" si="124">IF((X19+AA19)&lt;($J$4/2),"低",IF((X19+AA19)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AH19" s="7" t="str">
+        <f t="shared" ref="AH19" si="125">IF((Y19+AB19)&lt;($J$4/2),"低",IF((Y19+AB19)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AI19" s="7" t="str">
+        <f t="shared" ref="AI19" si="126">IF((Z19+AC19)&lt;($J$4/2),"低",IF((Z19+AC19)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" s="7" customFormat="1">
+      <c r="D20" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="7">
+        <v>52</v>
+      </c>
+      <c r="F20" s="7">
+        <v>70</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H20" s="7">
+        <v>35</v>
+      </c>
+      <c r="I20" s="7">
+        <v>7</v>
+      </c>
+      <c r="J20" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" ref="L20" si="127">E20*I20</f>
+        <v>364</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" ref="M20" si="128">E20*J20</f>
+        <v>546</v>
+      </c>
+      <c r="N20" s="7">
+        <f t="shared" ref="N20" si="129">E20*K20</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="7">
+        <f t="shared" ref="O20" si="130">F20*I20</f>
+        <v>490</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" ref="P20" si="131">F20*J20</f>
+        <v>735</v>
+      </c>
+      <c r="Q20" s="7">
+        <f t="shared" ref="Q20" si="132">F20*K20</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="7">
+        <f t="shared" ref="R20" si="133">H20*I20</f>
+        <v>245</v>
+      </c>
+      <c r="S20" s="7">
+        <f t="shared" ref="S20" si="134">H20*J20</f>
+        <v>367.5</v>
+      </c>
+      <c r="T20" s="7">
+        <f t="shared" ref="T20" si="135">H20*K20</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="4">
+        <f t="shared" ref="U20" si="136">L20*$G$3/$E$3</f>
+        <v>0.17975308641975307</v>
+      </c>
+      <c r="V20" s="4">
+        <f t="shared" ref="V20" si="137">M20*$G$3/$E$3</f>
+        <v>0.26962962962962961</v>
+      </c>
+      <c r="W20" s="4">
+        <f t="shared" ref="W20" si="138">N20*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X20" s="4">
+        <f t="shared" ref="X20" si="139">R20*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.12098765432098765</v>
+      </c>
+      <c r="Y20" s="4">
+        <f t="shared" ref="Y20" si="140">S20*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.18148148148148147</v>
+      </c>
+      <c r="Z20" s="4">
+        <f t="shared" ref="Z20" si="141">T20*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="4">
+        <f t="shared" ref="AA20" si="142">O20*$G$3/$E$3</f>
+        <v>0.24197530864197531</v>
+      </c>
+      <c r="AB20" s="4">
+        <f t="shared" ref="AB20" si="143">P20*$G$3/$E$3</f>
+        <v>0.36296296296296293</v>
+      </c>
+      <c r="AC20" s="4">
+        <f t="shared" ref="AC20" si="144">Q20*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="7" t="str">
+        <f t="shared" ref="AD20" si="145">IF((U20+X20)&lt;($J$4/2),"低",IF((U20+X20)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AE20" s="7" t="str">
+        <f t="shared" ref="AE20" si="146">IF((V20+Y20)&lt;($J$4/2),"低",IF((V20+Y20)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AF20" s="7" t="str">
+        <f t="shared" ref="AF20" si="147">IF((W20+Z20)&lt;($J$4/2),"低",IF((W20+Z20)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG20" s="7" t="str">
+        <f t="shared" ref="AG20" si="148">IF((X20+AA20)&lt;($J$4/2),"低",IF((X20+AA20)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH20" s="7" t="str">
+        <f t="shared" ref="AH20" si="149">IF((Y20+AB20)&lt;($J$4/2),"低",IF((Y20+AB20)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI20" s="7" t="str">
+        <f t="shared" ref="AI20" si="150">IF((Z20+AC20)&lt;($J$4/2),"低",IF((Z20+AC20)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" s="7" customFormat="1">
+      <c r="D21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="7">
+        <v>52</v>
+      </c>
+      <c r="F21" s="7">
+        <v>70</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H21" s="7">
+        <v>35</v>
+      </c>
+      <c r="I21" s="7">
+        <v>7</v>
+      </c>
+      <c r="J21" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" ref="L21" si="151">E21*I21</f>
+        <v>364</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" ref="M21" si="152">E21*J21</f>
+        <v>546</v>
+      </c>
+      <c r="N21" s="7">
+        <f t="shared" ref="N21" si="153">E21*K21</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="7">
+        <f t="shared" ref="O21" si="154">F21*I21</f>
+        <v>490</v>
+      </c>
+      <c r="P21" s="7">
+        <f t="shared" ref="P21" si="155">F21*J21</f>
+        <v>735</v>
+      </c>
+      <c r="Q21" s="7">
+        <f t="shared" ref="Q21" si="156">F21*K21</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" ref="R21" si="157">H21*I21</f>
+        <v>245</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" ref="S21" si="158">H21*J21</f>
+        <v>367.5</v>
+      </c>
+      <c r="T21" s="7">
+        <f t="shared" ref="T21" si="159">H21*K21</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" ref="U21" si="160">L21*$G$3/$E$3</f>
+        <v>0.17975308641975307</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" ref="V21" si="161">M21*$G$3/$E$3</f>
+        <v>0.26962962962962961</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" ref="W21" si="162">N21*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" ref="X21" si="163">R21*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.12098765432098765</v>
+      </c>
+      <c r="Y21" s="4">
+        <f t="shared" ref="Y21" si="164">S21*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.18148148148148147</v>
+      </c>
+      <c r="Z21" s="4">
+        <f t="shared" ref="Z21" si="165">T21*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="4">
+        <f t="shared" ref="AA21" si="166">O21*$G$3/$E$3</f>
+        <v>0.24197530864197531</v>
+      </c>
+      <c r="AB21" s="4">
+        <f t="shared" ref="AB21" si="167">P21*$G$3/$E$3</f>
+        <v>0.36296296296296293</v>
+      </c>
+      <c r="AC21" s="4">
+        <f t="shared" ref="AC21" si="168">Q21*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="7" t="str">
+        <f t="shared" ref="AD21" si="169">IF((U21+X21)&lt;($J$4/2),"低",IF((U21+X21)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AE21" s="7" t="str">
+        <f t="shared" ref="AE21" si="170">IF((V21+Y21)&lt;($J$4/2),"低",IF((V21+Y21)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AF21" s="7" t="str">
+        <f t="shared" ref="AF21" si="171">IF((W21+Z21)&lt;($J$4/2),"低",IF((W21+Z21)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG21" s="7" t="str">
+        <f t="shared" ref="AG21" si="172">IF((X21+AA21)&lt;($J$4/2),"低",IF((X21+AA21)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH21" s="7" t="str">
+        <f t="shared" ref="AH21" si="173">IF((Y21+AB21)&lt;($J$4/2),"低",IF((Y21+AB21)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI21" s="7" t="str">
+        <f t="shared" ref="AI21" si="174">IF((Z21+AC21)&lt;($J$4/2),"低",IF((Z21+AC21)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" s="7" customFormat="1">
+      <c r="D22" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="7">
+        <v>52</v>
+      </c>
+      <c r="F22" s="7">
+        <v>70</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="7">
+        <v>40</v>
+      </c>
+      <c r="I22" s="7">
+        <v>7</v>
+      </c>
+      <c r="J22" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K22" s="7">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7">
+        <f t="shared" ref="L22" si="175">E22*I22</f>
+        <v>364</v>
+      </c>
+      <c r="M22" s="7">
+        <f t="shared" ref="M22" si="176">E22*J22</f>
+        <v>546</v>
+      </c>
+      <c r="N22" s="7">
+        <f t="shared" ref="N22" si="177">E22*K22</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" ref="O22" si="178">F22*I22</f>
+        <v>490</v>
+      </c>
+      <c r="P22" s="7">
+        <f t="shared" ref="P22" si="179">F22*J22</f>
+        <v>735</v>
+      </c>
+      <c r="Q22" s="7">
+        <f t="shared" ref="Q22" si="180">F22*K22</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="7">
+        <f t="shared" ref="R22" si="181">H22*I22</f>
+        <v>280</v>
+      </c>
+      <c r="S22" s="7">
+        <f t="shared" ref="S22" si="182">H22*J22</f>
+        <v>420</v>
+      </c>
+      <c r="T22" s="7">
+        <f t="shared" ref="T22" si="183">H22*K22</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" ref="U22" si="184">L22*$G$3/$E$3</f>
+        <v>0.17975308641975307</v>
+      </c>
+      <c r="V22" s="4">
+        <f t="shared" ref="V22" si="185">M22*$G$3/$E$3</f>
+        <v>0.26962962962962961</v>
+      </c>
+      <c r="W22" s="4">
+        <f t="shared" ref="W22" si="186">N22*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="4">
+        <f t="shared" ref="X22" si="187">R22*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.13827160493827159</v>
+      </c>
+      <c r="Y22" s="4">
+        <f t="shared" ref="Y22" si="188">S22*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.2074074074074074</v>
+      </c>
+      <c r="Z22" s="4">
+        <f t="shared" ref="Z22" si="189">T22*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="4">
+        <f t="shared" ref="AA22" si="190">O22*$G$3/$E$3</f>
+        <v>0.24197530864197531</v>
+      </c>
+      <c r="AB22" s="4">
+        <f t="shared" ref="AB22" si="191">P22*$G$3/$E$3</f>
+        <v>0.36296296296296293</v>
+      </c>
+      <c r="AC22" s="4">
+        <f t="shared" ref="AC22" si="192">Q22*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="7" t="str">
+        <f t="shared" ref="AD22" si="193">IF((U22+X22)&lt;($J$4/2),"低",IF((U22+X22)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AE22" s="7" t="str">
+        <f t="shared" ref="AE22" si="194">IF((V22+Y22)&lt;($J$4/2),"低",IF((V22+Y22)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AF22" s="7" t="str">
+        <f t="shared" ref="AF22" si="195">IF((W22+Z22)&lt;($J$4/2),"低",IF((W22+Z22)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG22" s="7" t="str">
+        <f t="shared" ref="AG22" si="196">IF((X22+AA22)&lt;($J$4/2),"低",IF((X22+AA22)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH22" s="7" t="str">
+        <f t="shared" ref="AH22" si="197">IF((Y22+AB22)&lt;($J$4/2),"低",IF((Y22+AB22)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI22" s="7" t="str">
+        <f t="shared" ref="AI22" si="198">IF((Z22+AC22)&lt;($J$4/2),"低",IF((Z22+AC22)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" s="7" customFormat="1">
+      <c r="D23" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="7">
+        <v>64</v>
+      </c>
+      <c r="F23" s="7">
+        <v>86</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H23" s="7">
+        <v>50</v>
+      </c>
+      <c r="I23" s="7">
+        <v>7</v>
+      </c>
+      <c r="J23" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K23" s="7">
+        <v>0</v>
+      </c>
+      <c r="L23" s="7">
+        <f t="shared" ref="L23" si="199">E23*I23</f>
+        <v>448</v>
+      </c>
+      <c r="M23" s="7">
+        <f t="shared" ref="M23" si="200">E23*J23</f>
+        <v>672</v>
+      </c>
+      <c r="N23" s="7">
+        <f t="shared" ref="N23" si="201">E23*K23</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="7">
+        <f t="shared" ref="O23" si="202">F23*I23</f>
+        <v>602</v>
+      </c>
+      <c r="P23" s="7">
+        <f t="shared" ref="P23" si="203">F23*J23</f>
+        <v>903</v>
+      </c>
+      <c r="Q23" s="7">
+        <f t="shared" ref="Q23" si="204">F23*K23</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="7">
+        <f t="shared" ref="R23" si="205">H23*I23</f>
+        <v>350</v>
+      </c>
+      <c r="S23" s="7">
+        <f t="shared" ref="S23" si="206">H23*J23</f>
+        <v>525</v>
+      </c>
+      <c r="T23" s="7">
+        <f t="shared" ref="T23" si="207">H23*K23</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="4">
+        <f t="shared" ref="U23" si="208">L23*$G$3/$E$3</f>
+        <v>0.22123456790123455</v>
+      </c>
+      <c r="V23" s="4">
+        <f t="shared" ref="V23" si="209">M23*$G$3/$E$3</f>
+        <v>0.33185185185185179</v>
+      </c>
+      <c r="W23" s="4">
+        <f t="shared" ref="W23" si="210">N23*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X23" s="4">
+        <f t="shared" ref="X23" si="211">R23*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.1728395061728395</v>
+      </c>
+      <c r="Y23" s="4">
+        <f t="shared" ref="Y23" si="212">S23*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="Z23" s="4">
+        <f t="shared" ref="Z23" si="213">T23*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="4">
+        <f t="shared" ref="AA23" si="214">O23*$G$3/$E$3</f>
+        <v>0.29728395061728391</v>
+      </c>
+      <c r="AB23" s="4">
+        <f t="shared" ref="AB23" si="215">P23*$G$3/$E$3</f>
+        <v>0.44592592592592589</v>
+      </c>
+      <c r="AC23" s="4">
+        <f t="shared" ref="AC23" si="216">Q23*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="7" t="str">
+        <f t="shared" ref="AD23" si="217">IF((U23+X23)&lt;($J$4/2),"低",IF((U23+X23)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AE23" s="7" t="str">
+        <f t="shared" ref="AE23" si="218">IF((V23+Y23)&lt;($J$4/2),"低",IF((V23+Y23)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AF23" s="7" t="str">
+        <f t="shared" ref="AF23" si="219">IF((W23+Z23)&lt;($J$4/2),"低",IF((W23+Z23)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG23" s="7" t="str">
+        <f t="shared" ref="AG23" si="220">IF((X23+AA23)&lt;($J$4/2),"低",IF((X23+AA23)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AH23" s="7" t="str">
+        <f t="shared" ref="AH23" si="221">IF((Y23+AB23)&lt;($J$4/2),"低",IF((Y23+AB23)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI23" s="7" t="str">
+        <f t="shared" ref="AI23" si="222">IF((Z23+AC23)&lt;($J$4/2),"低",IF((Z23+AC23)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" s="7" customFormat="1">
+      <c r="D24" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="7">
+        <v>81</v>
+      </c>
+      <c r="F24" s="7">
+        <v>108</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H24" s="7">
+        <v>70</v>
+      </c>
+      <c r="I24" s="7">
+        <v>7</v>
+      </c>
+      <c r="J24" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7">
+        <f t="shared" ref="L24" si="223">E24*I24</f>
+        <v>567</v>
+      </c>
+      <c r="M24" s="7">
+        <f t="shared" ref="M24" si="224">E24*J24</f>
+        <v>850.5</v>
+      </c>
+      <c r="N24" s="7">
+        <f t="shared" ref="N24" si="225">E24*K24</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="7">
+        <f t="shared" ref="O24" si="226">F24*I24</f>
+        <v>756</v>
+      </c>
+      <c r="P24" s="7">
+        <f t="shared" ref="P24" si="227">F24*J24</f>
+        <v>1134</v>
+      </c>
+      <c r="Q24" s="7">
+        <f t="shared" ref="Q24" si="228">F24*K24</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="7">
+        <f t="shared" ref="R24" si="229">H24*I24</f>
+        <v>490</v>
+      </c>
+      <c r="S24" s="7">
+        <f t="shared" ref="S24" si="230">H24*J24</f>
+        <v>735</v>
+      </c>
+      <c r="T24" s="7">
+        <f t="shared" ref="T24" si="231">H24*K24</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="4">
+        <f t="shared" ref="U24" si="232">L24*$G$3/$E$3</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V24" s="4">
+        <f t="shared" ref="V24" si="233">M24*$G$3/$E$3</f>
+        <v>0.42</v>
+      </c>
+      <c r="W24" s="4">
+        <f t="shared" ref="W24" si="234">N24*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X24" s="4">
+        <f t="shared" ref="X24" si="235">R24*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.24197530864197531</v>
+      </c>
+      <c r="Y24" s="4">
+        <f t="shared" ref="Y24" si="236">S24*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.36296296296296293</v>
+      </c>
+      <c r="Z24" s="4">
+        <f t="shared" ref="Z24" si="237">T24*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="4">
+        <f t="shared" ref="AA24" si="238">O24*$G$3/$E$3</f>
+        <v>0.37333333333333335</v>
+      </c>
+      <c r="AB24" s="4">
+        <f t="shared" ref="AB24" si="239">P24*$G$3/$E$3</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC24" s="4">
+        <f t="shared" ref="AC24" si="240">Q24*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="7" t="str">
+        <f t="shared" ref="AD24" si="241">IF((U24+X24)&lt;($J$4/2),"低",IF((U24+X24)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AE24" s="7" t="str">
+        <f t="shared" ref="AE24" si="242">IF((V24+Y24)&lt;($J$4/2),"低",IF((V24+Y24)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AF24" s="7" t="str">
+        <f t="shared" ref="AF24" si="243">IF((W24+Z24)&lt;($J$4/2),"低",IF((W24+Z24)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG24" s="7" t="str">
+        <f t="shared" ref="AG24" si="244">IF((X24+AA24)&lt;($J$4/2),"低",IF((X24+AA24)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AH24" s="7" t="str">
+        <f t="shared" ref="AH24" si="245">IF((Y24+AB24)&lt;($J$4/2),"低",IF((Y24+AB24)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI24" s="7" t="str">
+        <f t="shared" ref="AI24" si="246">IF((Z24+AC24)&lt;($J$4/2),"低",IF((Z24+AC24)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" s="7" customFormat="1">
+      <c r="D25" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E25" s="7">
+        <v>52</v>
+      </c>
+      <c r="F25" s="7">
+        <v>70</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H25" s="7">
+        <v>40</v>
+      </c>
+      <c r="I25" s="7">
+        <v>7</v>
+      </c>
+      <c r="J25" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0</v>
+      </c>
+      <c r="L25" s="7">
+        <f t="shared" ref="L25" si="247">E25*I25</f>
+        <v>364</v>
+      </c>
+      <c r="M25" s="7">
+        <f t="shared" ref="M25" si="248">E25*J25</f>
+        <v>546</v>
+      </c>
+      <c r="N25" s="7">
+        <f t="shared" ref="N25" si="249">E25*K25</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" ref="O25" si="250">F25*I25</f>
+        <v>490</v>
+      </c>
+      <c r="P25" s="7">
+        <f t="shared" ref="P25" si="251">F25*J25</f>
+        <v>735</v>
+      </c>
+      <c r="Q25" s="7">
+        <f t="shared" ref="Q25" si="252">F25*K25</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="7">
+        <f t="shared" ref="R25" si="253">H25*I25</f>
+        <v>280</v>
+      </c>
+      <c r="S25" s="7">
+        <f t="shared" ref="S25" si="254">H25*J25</f>
+        <v>420</v>
+      </c>
+      <c r="T25" s="7">
+        <f t="shared" ref="T25" si="255">H25*K25</f>
+        <v>0</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" ref="U25" si="256">L25*$G$3/$E$3</f>
+        <v>0.17975308641975307</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" ref="V25" si="257">M25*$G$3/$E$3</f>
+        <v>0.26962962962962961</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" ref="W25" si="258">N25*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X25" s="4">
+        <f t="shared" ref="X25" si="259">R25*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.13827160493827159</v>
+      </c>
+      <c r="Y25" s="4">
+        <f t="shared" ref="Y25" si="260">S25*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.2074074074074074</v>
+      </c>
+      <c r="Z25" s="4">
+        <f t="shared" ref="Z25" si="261">T25*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="4">
+        <f t="shared" ref="AA25" si="262">O25*$G$3/$E$3</f>
+        <v>0.24197530864197531</v>
+      </c>
+      <c r="AB25" s="4">
+        <f t="shared" ref="AB25" si="263">P25*$G$3/$E$3</f>
+        <v>0.36296296296296293</v>
+      </c>
+      <c r="AC25" s="4">
+        <f t="shared" ref="AC25" si="264">Q25*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD25" s="7" t="str">
+        <f t="shared" ref="AD25" si="265">IF((U25+X25)&lt;($J$4/2),"低",IF((U25+X25)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AE25" s="7" t="str">
+        <f t="shared" ref="AE25" si="266">IF((V25+Y25)&lt;($J$4/2),"低",IF((V25+Y25)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AF25" s="7" t="str">
+        <f t="shared" ref="AF25" si="267">IF((W25+Z25)&lt;($J$4/2),"低",IF((W25+Z25)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG25" s="7" t="str">
+        <f t="shared" ref="AG25" si="268">IF((X25+AA25)&lt;($J$4/2),"低",IF((X25+AA25)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH25" s="7" t="str">
+        <f t="shared" ref="AH25" si="269">IF((Y25+AB25)&lt;($J$4/2),"低",IF((Y25+AB25)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI25" s="7" t="str">
+        <f t="shared" ref="AI25" si="270">IF((Z25+AC25)&lt;($J$4/2),"低",IF((Z25+AC25)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" s="7" customFormat="1">
+      <c r="D26" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="7">
+        <v>64</v>
+      </c>
+      <c r="F26" s="7">
+        <v>86</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H26" s="7">
+        <v>40</v>
+      </c>
+      <c r="I26" s="7">
+        <v>7</v>
+      </c>
+      <c r="J26" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="K26" s="7">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7">
+        <f t="shared" ref="L26" si="271">E26*I26</f>
+        <v>448</v>
+      </c>
+      <c r="M26" s="7">
+        <f t="shared" ref="M26" si="272">E26*J26</f>
+        <v>672</v>
+      </c>
+      <c r="N26" s="7">
+        <f t="shared" ref="N26" si="273">E26*K26</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" ref="O26" si="274">F26*I26</f>
+        <v>602</v>
+      </c>
+      <c r="P26" s="7">
+        <f t="shared" ref="P26" si="275">F26*J26</f>
+        <v>903</v>
+      </c>
+      <c r="Q26" s="7">
+        <f t="shared" ref="Q26" si="276">F26*K26</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="7">
+        <f t="shared" ref="R26" si="277">H26*I26</f>
+        <v>280</v>
+      </c>
+      <c r="S26" s="7">
+        <f t="shared" ref="S26" si="278">H26*J26</f>
+        <v>420</v>
+      </c>
+      <c r="T26" s="7">
+        <f t="shared" ref="T26" si="279">H26*K26</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="4">
+        <f t="shared" ref="U26" si="280">L26*$G$3/$E$3</f>
+        <v>0.22123456790123455</v>
+      </c>
+      <c r="V26" s="4">
+        <f t="shared" ref="V26" si="281">M26*$G$3/$E$3</f>
+        <v>0.33185185185185179</v>
+      </c>
+      <c r="W26" s="4">
+        <f t="shared" ref="W26" si="282">N26*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="X26" s="4">
+        <f t="shared" ref="X26" si="283">R26*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.13827160493827159</v>
+      </c>
+      <c r="Y26" s="4">
+        <f t="shared" ref="Y26" si="284">S26*$G$3*(1-$H$3)/$E$3</f>
+        <v>0.2074074074074074</v>
+      </c>
+      <c r="Z26" s="4">
+        <f t="shared" ref="Z26" si="285">T26*$G$3*(1-$H$3)/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="4">
+        <f t="shared" ref="AA26" si="286">O26*$G$3/$E$3</f>
+        <v>0.29728395061728391</v>
+      </c>
+      <c r="AB26" s="4">
+        <f t="shared" ref="AB26" si="287">P26*$G$3/$E$3</f>
+        <v>0.44592592592592589</v>
+      </c>
+      <c r="AC26" s="4">
+        <f t="shared" ref="AC26" si="288">Q26*$G$3/$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="7" t="str">
+        <f t="shared" ref="AD26" si="289">IF((U26+X26)&lt;($J$4/2),"低",IF((U26+X26)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AE26" s="7" t="str">
+        <f t="shared" ref="AE26" si="290">IF((V26+Y26)&lt;($J$4/2),"低",IF((V26+Y26)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AF26" s="7" t="str">
+        <f t="shared" ref="AF26" si="291">IF((W26+Z26)&lt;($J$4/2),"低",IF((W26+Z26)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+      <c r="AG26" s="7" t="str">
+        <f t="shared" ref="AG26" si="292">IF((X26+AA26)&lt;($J$4/2),"低",IF((X26+AA26)&gt;$J$4,"高","中"))</f>
+        <v>中</v>
+      </c>
+      <c r="AH26" s="7" t="str">
+        <f t="shared" ref="AH26" si="293">IF((Y26+AB26)&lt;($J$4/2),"低",IF((Y26+AB26)&gt;$J$4,"高","中"))</f>
+        <v>高</v>
+      </c>
+      <c r="AI26" s="7" t="str">
+        <f t="shared" ref="AI26" si="294">IF((Z26+AC26)&lt;($J$4/2),"低",IF((Z26+AC26)&gt;$J$4,"高","中"))</f>
+        <v>低</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35">
       <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
@@ -2461,15 +3852,15 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:35">
       <c r="A28" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
@@ -2481,15 +3872,15 @@
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:35">
       <c r="A29" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
@@ -2501,15 +3892,15 @@
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:35">
       <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
@@ -2521,15 +3912,15 @@
       <c r="AB30" s="4"/>
       <c r="AC30" s="4"/>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:35">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
@@ -2541,15 +3932,15 @@
       <c r="AB31" s="4"/>
       <c r="AC31" s="4"/>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:35">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
@@ -2563,13 +3954,13 @@
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
@@ -2583,13 +3974,13 @@
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
@@ -2603,13 +3994,13 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
@@ -2623,13 +4014,13 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
@@ -2643,13 +4034,13 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
@@ -2663,13 +4054,13 @@
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
@@ -2683,13 +4074,13 @@
     </row>
     <row r="39" spans="1:29">
       <c r="A39" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
@@ -2703,13 +4094,13 @@
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
@@ -2723,13 +4114,13 @@
     </row>
     <row r="41" spans="1:29">
       <c r="A41" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
@@ -2743,13 +4134,13 @@
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
@@ -2763,13 +4154,13 @@
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
@@ -2783,13 +4174,13 @@
     </row>
     <row r="44" spans="1:29">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
@@ -2803,13 +4194,13 @@
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
@@ -2823,13 +4214,13 @@
     </row>
     <row r="46" spans="1:29">
       <c r="A46" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
@@ -2843,13 +4234,13 @@
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
@@ -2863,13 +4254,13 @@
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
@@ -2883,13 +4274,13 @@
     </row>
     <row r="49" spans="1:29">
       <c r="A49" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
@@ -2903,13 +4294,13 @@
     </row>
     <row r="50" spans="1:29">
       <c r="A50" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
@@ -2923,13 +4314,13 @@
     </row>
     <row r="51" spans="1:29">
       <c r="A51" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="U51" s="4"/>
       <c r="V51" s="4"/>
@@ -2943,13 +4334,13 @@
     </row>
     <row r="52" spans="1:29">
       <c r="A52" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="U52" s="4"/>
       <c r="V52" s="4"/>
@@ -2966,10 +4357,10 @@
         <v>43</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="U53" s="4"/>
       <c r="V53" s="4"/>
@@ -2986,10 +4377,10 @@
         <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="U54" s="4"/>
       <c r="V54" s="4"/>
@@ -3006,10 +4397,10 @@
         <v>43</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="U55" s="4"/>
       <c r="V55" s="4"/>
@@ -3026,10 +4417,10 @@
         <v>43</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="U56" s="4"/>
       <c r="V56" s="4"/>
@@ -3046,10 +4437,10 @@
         <v>43</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="U57" s="4"/>
       <c r="V57" s="4"/>
@@ -3066,10 +4457,10 @@
         <v>43</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="U58" s="4"/>
       <c r="V58" s="4"/>
@@ -3086,10 +4477,10 @@
         <v>43</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="U59" s="4"/>
       <c r="V59" s="4"/>
@@ -3106,10 +4497,10 @@
         <v>43</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="U60" s="4"/>
       <c r="V60" s="4"/>
@@ -3123,13 +4514,13 @@
     </row>
     <row r="61" spans="1:29">
       <c r="A61" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="U61" s="4"/>
       <c r="V61" s="4"/>
@@ -3143,13 +4534,13 @@
     </row>
     <row r="62" spans="1:29">
       <c r="A62" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="U62" s="4"/>
       <c r="V62" s="4"/>
@@ -3163,13 +4554,13 @@
     </row>
     <row r="63" spans="1:29">
       <c r="A63" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="U63" s="4"/>
       <c r="V63" s="4"/>
@@ -3183,13 +4574,13 @@
     </row>
     <row r="64" spans="1:29">
       <c r="A64" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="U64" s="4"/>
       <c r="V64" s="4"/>
@@ -3203,13 +4594,13 @@
     </row>
     <row r="65" spans="1:29">
       <c r="A65" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="U65" s="4"/>
       <c r="V65" s="4"/>
@@ -3223,13 +4614,13 @@
     </row>
     <row r="66" spans="1:29">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="U66" s="4"/>
       <c r="V66" s="4"/>
@@ -3243,13 +4634,13 @@
     </row>
     <row r="67" spans="1:29">
       <c r="A67" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="U67" s="4"/>
       <c r="V67" s="4"/>
@@ -3263,13 +4654,13 @@
     </row>
     <row r="68" spans="1:29">
       <c r="A68" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U68" s="4"/>
       <c r="V68" s="4"/>
@@ -3283,13 +4674,13 @@
     </row>
     <row r="69" spans="1:29">
       <c r="A69" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="U69" s="4"/>
       <c r="V69" s="4"/>
@@ -3303,13 +4694,13 @@
     </row>
     <row r="70" spans="1:29">
       <c r="A70" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="U70" s="4"/>
       <c r="V70" s="4"/>
@@ -3323,13 +4714,13 @@
     </row>
     <row r="71" spans="1:29">
       <c r="A71" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="U71" s="4"/>
       <c r="V71" s="4"/>
@@ -3343,13 +4734,13 @@
     </row>
     <row r="72" spans="1:29">
       <c r="A72" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="U72" s="4"/>
       <c r="V72" s="4"/>
@@ -3363,13 +4754,13 @@
     </row>
     <row r="73" spans="1:29">
       <c r="A73" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="U73" s="4"/>
       <c r="V73" s="4"/>
@@ -3383,13 +4774,13 @@
     </row>
     <row r="74" spans="1:29">
       <c r="A74" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="U74" s="4"/>
       <c r="V74" s="4"/>
@@ -3406,10 +4797,10 @@
         <v>67</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="U75" s="4"/>
       <c r="V75" s="4"/>
@@ -3426,10 +4817,10 @@
         <v>67</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="U76" s="4"/>
       <c r="V76" s="4"/>
@@ -3446,10 +4837,10 @@
         <v>67</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="U77" s="4"/>
       <c r="V77" s="4"/>
@@ -3466,10 +4857,10 @@
         <v>67</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="U78" s="4"/>
       <c r="V78" s="4"/>
@@ -3486,10 +4877,10 @@
         <v>67</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="U79" s="4"/>
       <c r="V79" s="4"/>
@@ -3506,10 +4897,10 @@
         <v>67</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="U80" s="4"/>
       <c r="V80" s="4"/>
@@ -3522,14 +4913,14 @@
       <c r="AC80" s="4"/>
     </row>
     <row r="81" spans="1:29">
-      <c r="A81" s="3" t="s">
-        <v>85</v>
+      <c r="A81" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="U81" s="4"/>
       <c r="V81" s="4"/>
@@ -3542,14 +4933,14 @@
       <c r="AC81" s="4"/>
     </row>
     <row r="82" spans="1:29">
-      <c r="A82" s="3" t="s">
-        <v>85</v>
+      <c r="A82" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="U82" s="4"/>
       <c r="V82" s="4"/>
@@ -3562,6 +4953,15 @@
       <c r="AC82" s="4"/>
     </row>
     <row r="83" spans="1:29">
+      <c r="A83" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="U83" s="4"/>
       <c r="V83" s="4"/>
       <c r="W83" s="4"/>
@@ -3573,6 +4973,15 @@
       <c r="AC83" s="4"/>
     </row>
     <row r="84" spans="1:29">
+      <c r="A84" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="U84" s="4"/>
       <c r="V84" s="4"/>
       <c r="W84" s="4"/>
@@ -3584,6 +4993,15 @@
       <c r="AC84" s="4"/>
     </row>
     <row r="85" spans="1:29">
+      <c r="A85" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="U85" s="4"/>
       <c r="V85" s="4"/>
       <c r="W85" s="4"/>
@@ -3595,6 +5013,15 @@
       <c r="AC85" s="4"/>
     </row>
     <row r="86" spans="1:29">
+      <c r="A86" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="U86" s="4"/>
       <c r="V86" s="4"/>
       <c r="W86" s="4"/>
@@ -3606,6 +5033,15 @@
       <c r="AC86" s="4"/>
     </row>
     <row r="87" spans="1:29">
+      <c r="A87" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U87" s="4"/>
       <c r="V87" s="4"/>
       <c r="W87" s="4"/>
@@ -3617,6 +5053,15 @@
       <c r="AC87" s="4"/>
     </row>
     <row r="88" spans="1:29">
+      <c r="A88" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="U88" s="4"/>
       <c r="V88" s="4"/>
       <c r="W88" s="4"/>
@@ -3628,6 +5073,15 @@
       <c r="AC88" s="4"/>
     </row>
     <row r="89" spans="1:29">
+      <c r="A89" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="U89" s="4"/>
       <c r="V89" s="4"/>
       <c r="W89" s="4"/>
@@ -3639,6 +5093,15 @@
       <c r="AC89" s="4"/>
     </row>
     <row r="90" spans="1:29">
+      <c r="A90" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="U90" s="4"/>
       <c r="V90" s="4"/>
       <c r="W90" s="4"/>
@@ -3650,6 +5113,15 @@
       <c r="AC90" s="4"/>
     </row>
     <row r="91" spans="1:29">
+      <c r="A91" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="U91" s="4"/>
       <c r="V91" s="4"/>
       <c r="W91" s="4"/>
@@ -3661,6 +5133,15 @@
       <c r="AC91" s="4"/>
     </row>
     <row r="92" spans="1:29">
+      <c r="A92" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="U92" s="4"/>
       <c r="V92" s="4"/>
       <c r="W92" s="4"/>
@@ -3672,6 +5153,15 @@
       <c r="AC92" s="4"/>
     </row>
     <row r="93" spans="1:29">
+      <c r="A93" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="U93" s="4"/>
       <c r="V93" s="4"/>
       <c r="W93" s="4"/>
@@ -6992,6 +8482,127 @@
       <c r="AA394" s="4"/>
       <c r="AB394" s="4"/>
       <c r="AC394" s="4"/>
+    </row>
+    <row r="395" spans="21:29">
+      <c r="U395" s="4"/>
+      <c r="V395" s="4"/>
+      <c r="W395" s="4"/>
+      <c r="X395" s="4"/>
+      <c r="Y395" s="4"/>
+      <c r="Z395" s="4"/>
+      <c r="AA395" s="4"/>
+      <c r="AB395" s="4"/>
+      <c r="AC395" s="4"/>
+    </row>
+    <row r="396" spans="21:29">
+      <c r="U396" s="4"/>
+      <c r="V396" s="4"/>
+      <c r="W396" s="4"/>
+      <c r="X396" s="4"/>
+      <c r="Y396" s="4"/>
+      <c r="Z396" s="4"/>
+      <c r="AA396" s="4"/>
+      <c r="AB396" s="4"/>
+      <c r="AC396" s="4"/>
+    </row>
+    <row r="397" spans="21:29">
+      <c r="U397" s="4"/>
+      <c r="V397" s="4"/>
+      <c r="W397" s="4"/>
+      <c r="X397" s="4"/>
+      <c r="Y397" s="4"/>
+      <c r="Z397" s="4"/>
+      <c r="AA397" s="4"/>
+      <c r="AB397" s="4"/>
+      <c r="AC397" s="4"/>
+    </row>
+    <row r="398" spans="21:29">
+      <c r="U398" s="4"/>
+      <c r="V398" s="4"/>
+      <c r="W398" s="4"/>
+      <c r="X398" s="4"/>
+      <c r="Y398" s="4"/>
+      <c r="Z398" s="4"/>
+      <c r="AA398" s="4"/>
+      <c r="AB398" s="4"/>
+      <c r="AC398" s="4"/>
+    </row>
+    <row r="399" spans="21:29">
+      <c r="U399" s="4"/>
+      <c r="V399" s="4"/>
+      <c r="W399" s="4"/>
+      <c r="X399" s="4"/>
+      <c r="Y399" s="4"/>
+      <c r="Z399" s="4"/>
+      <c r="AA399" s="4"/>
+      <c r="AB399" s="4"/>
+      <c r="AC399" s="4"/>
+    </row>
+    <row r="400" spans="21:29">
+      <c r="U400" s="4"/>
+      <c r="V400" s="4"/>
+      <c r="W400" s="4"/>
+      <c r="X400" s="4"/>
+      <c r="Y400" s="4"/>
+      <c r="Z400" s="4"/>
+      <c r="AA400" s="4"/>
+      <c r="AB400" s="4"/>
+      <c r="AC400" s="4"/>
+    </row>
+    <row r="401" spans="21:29">
+      <c r="U401" s="4"/>
+      <c r="V401" s="4"/>
+      <c r="W401" s="4"/>
+      <c r="X401" s="4"/>
+      <c r="Y401" s="4"/>
+      <c r="Z401" s="4"/>
+      <c r="AA401" s="4"/>
+      <c r="AB401" s="4"/>
+      <c r="AC401" s="4"/>
+    </row>
+    <row r="402" spans="21:29">
+      <c r="U402" s="4"/>
+      <c r="V402" s="4"/>
+      <c r="W402" s="4"/>
+      <c r="X402" s="4"/>
+      <c r="Y402" s="4"/>
+      <c r="Z402" s="4"/>
+      <c r="AA402" s="4"/>
+      <c r="AB402" s="4"/>
+      <c r="AC402" s="4"/>
+    </row>
+    <row r="403" spans="21:29">
+      <c r="U403" s="4"/>
+      <c r="V403" s="4"/>
+      <c r="W403" s="4"/>
+      <c r="X403" s="4"/>
+      <c r="Y403" s="4"/>
+      <c r="Z403" s="4"/>
+      <c r="AA403" s="4"/>
+      <c r="AB403" s="4"/>
+      <c r="AC403" s="4"/>
+    </row>
+    <row r="404" spans="21:29">
+      <c r="U404" s="4"/>
+      <c r="V404" s="4"/>
+      <c r="W404" s="4"/>
+      <c r="X404" s="4"/>
+      <c r="Y404" s="4"/>
+      <c r="Z404" s="4"/>
+      <c r="AA404" s="4"/>
+      <c r="AB404" s="4"/>
+      <c r="AC404" s="4"/>
+    </row>
+    <row r="405" spans="21:29">
+      <c r="U405" s="4"/>
+      <c r="V405" s="4"/>
+      <c r="W405" s="4"/>
+      <c r="X405" s="4"/>
+      <c r="Y405" s="4"/>
+      <c r="Z405" s="4"/>
+      <c r="AA405" s="4"/>
+      <c r="AB405" s="4"/>
+      <c r="AC405" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>